<commit_message>
Updating SAP workflows - 26-10-2022 - 1:40pm
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SYS-QAUPBOT2\.nuget\packages\scenario4and6.performer\3.5.1\lib\net45\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DBAB2BA-8F81-4BC4-BC80-B5B17443C2C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD92B035-3A1F-4AD9-8A35-5CA7D3314ED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="26010" windowHeight="20160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="109">
   <si>
     <t>Name</t>
   </si>
@@ -340,13 +340,25 @@
   </si>
   <si>
     <t>C:\Program Files (x86)\SAP\NWBC70\nwbc.exe</t>
+  </si>
+  <si>
+    <t>TimeOut_5second</t>
+  </si>
+  <si>
+    <t>Timeout equals to 5 second</t>
+  </si>
+  <si>
+    <t>TimeOut_10second</t>
+  </si>
+  <si>
+    <t>Timeout equals to 10 second</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -390,6 +402,11 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -417,7 +434,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -442,6 +459,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2002,10 +2020,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z990"/>
+  <dimension ref="A1:Z992"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2207,108 +2225,128 @@
         <v>98</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="45">
-      <c r="A19" t="s">
+    <row r="19" spans="1:3" s="16" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A19" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="B19" s="16">
+        <v>5000</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" s="16" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A20" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="B20" s="16">
+        <v>10000</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="45">
+      <c r="A21" t="s">
         <v>39</v>
       </c>
-      <c r="B19" t="b">
+      <c r="B21" t="b">
         <v>0</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C21" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="21" spans="1:3" s="11" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A21" s="9" t="s">
+    <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:3" s="11" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A23" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-    </row>
-    <row r="22" spans="1:3" s="11" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A22" s="11" t="s">
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+    </row>
+    <row r="24" spans="1:3" s="11" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A24" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B24" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C24" s="12" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="2"/>
-    </row>
-    <row r="24" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A24" s="14" t="s">
+    <row r="25" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A25" s="7"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="2"/>
+    </row>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A26" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
-    </row>
-    <row r="25" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A25" s="11" t="s">
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+    </row>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A27" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="13" t="s">
+      <c r="B27" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C27" s="13" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="27" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A27" s="15" t="s">
+    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A29" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="B27" s="15"/>
-      <c r="C27" s="15"/>
-    </row>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A28" t="s">
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
+    </row>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A30" t="s">
         <v>100</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B30" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A30" s="15" t="s">
+    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A32" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="B30" s="15"/>
-      <c r="C30" s="15"/>
-    </row>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A31" t="s">
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
+    </row>
+    <row r="33" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A33" t="s">
         <v>103</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B33" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="33" ht="14.25" customHeight="1"/>
-    <row r="34" ht="14.25" customHeight="1"/>
-    <row r="35" ht="14.25" customHeight="1"/>
-    <row r="36" ht="14.25" customHeight="1"/>
-    <row r="37" ht="14.25" customHeight="1"/>
-    <row r="38" ht="14.25" customHeight="1"/>
-    <row r="39" ht="14.25" customHeight="1"/>
-    <row r="40" ht="14.25" customHeight="1"/>
-    <row r="41" ht="14.25" customHeight="1"/>
-    <row r="42" ht="14.25" customHeight="1"/>
-    <row r="43" ht="14.25" customHeight="1"/>
-    <row r="44" ht="14.25" customHeight="1"/>
-    <row r="45" ht="14.25" customHeight="1"/>
-    <row r="46" ht="14.25" customHeight="1"/>
-    <row r="47" ht="14.25" customHeight="1"/>
-    <row r="48" ht="14.25" customHeight="1"/>
+    <row r="34" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="35" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="36" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="37" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="38" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="39" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="40" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="41" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="42" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="43" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="44" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="45" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="46" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="47" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="48" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="49" ht="14.25" customHeight="1"/>
     <row r="50" ht="14.25" customHeight="1"/>
     <row r="51" ht="14.25" customHeight="1"/>
@@ -3251,6 +3289,8 @@
     <row r="988" ht="14.25" customHeight="1"/>
     <row r="989" ht="14.25" customHeight="1"/>
     <row r="990" ht="14.25" customHeight="1"/>
+    <row r="991" ht="14.25" customHeight="1"/>
+    <row r="992" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updating SAP workflows - 02-11-2022 - 11:00am
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SYS-QAUPBOT2\.nuget\packages\scenario4and6.performer\3.5.1\lib\net45\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3FB628E-3767-4315-9F83-18C9382C0045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70045E2E-236D-466F-946D-59D13E7F80AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="26010" windowHeight="20160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2029,7 +2029,7 @@
   <dimension ref="A1:Z993"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>